<commit_message>
Changed 4 tables in BMI-platelet chapter to a figure. Made changes from Nic's comments
</commit_message>
<xml_diff>
--- a/index/figure/BMI_platelets/BMI_platelets_supp_tables.xlsx
+++ b/index/figure/BMI_platelets/BMI_platelets_supp_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/lg14289_bristol_ac_uk/Documents/PhD/Main project/Thesis/index/figure/BMI_platelets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="518" documentId="8_{3A69ACBE-72F1-F24A-B1A9-6DAC356E931A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91B1A0C9-F0F5-DF4D-AFFC-7714116A7D2E}"/>
+  <xr:revisionPtr revIDLastSave="520" documentId="8_{3A69ACBE-72F1-F24A-B1A9-6DAC356E931A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A99D37A9-DE94-1D43-8D75-612D08282C58}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="11640" activeTab="6" xr2:uid="{BE97C42A-C506-DC4E-8BCC-02F8B6F9778C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="11640" activeTab="5" xr2:uid="{BE97C42A-C506-DC4E-8BCC-02F8B6F9778C}"/>
   </bookViews>
   <sheets>
     <sheet name="Supp Table 1" sheetId="13" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="60">
   <si>
     <t>Variable</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Beta coefficient is the change in platelet traits (SDs) per unit change in smoking category (1 = never, 2 = previous, 3 = current)</t>
   </si>
   <si>
-    <t>95%CI</t>
-  </si>
-  <si>
     <t>Lower_95%</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
   </si>
   <si>
     <t>Beta coefficient is the change in platelet traits in SDs per unit increase in alcohol consumption (1=Rarely , 2= Less than weekly, 3=One or two weekly, 4= 3-5 weekly or every day)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beta_coefficient </t>
   </si>
   <si>
     <t>P-LCR</t>
@@ -622,7 +616,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -630,7 +624,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
@@ -645,27 +639,27 @@
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>27997</v>
@@ -700,10 +694,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>29682</v>
@@ -738,10 +732,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>27268</v>
@@ -776,10 +770,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>29721</v>
@@ -814,10 +808,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7">
         <v>27255</v>
@@ -852,10 +846,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>27998</v>
@@ -890,10 +884,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>29721</v>
@@ -928,10 +922,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>29708</v>
@@ -966,10 +960,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>27255</v>
@@ -1004,10 +998,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>29721</v>
@@ -1042,10 +1036,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>30788</v>
@@ -1080,10 +1074,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>27994</v>
@@ -1118,12 +1112,12 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1156,7 +1150,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1176,7 +1170,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -1263,7 +1257,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>29538</v>
@@ -1349,7 +1343,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="J2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1360,7 +1354,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1368,7 +1362,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -1383,24 +1377,24 @@
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>29721</v>
@@ -1432,10 +1426,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>29721</v>
@@ -1467,10 +1461,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>29721</v>
@@ -1502,10 +1496,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>27997</v>
@@ -1537,10 +1531,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>29682</v>
@@ -1572,10 +1566,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>27994</v>
@@ -1607,10 +1601,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>27268</v>
@@ -1642,10 +1636,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>30788</v>
@@ -1677,10 +1671,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>27255</v>
@@ -1712,10 +1706,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>27998</v>
@@ -1747,10 +1741,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>29708</v>
@@ -1782,10 +1776,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14">
         <v>27255</v>
@@ -1817,7 +1811,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1829,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B665966C-0A72-914E-83AD-C27DA55D2694}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1842,7 +1836,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -1851,7 +1845,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -1866,24 +1860,24 @@
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>27268</v>
@@ -1915,10 +1909,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>29682</v>
@@ -1950,10 +1944,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>27997</v>
@@ -1985,10 +1979,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>27255</v>
@@ -2020,10 +2014,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>29708</v>
@@ -2055,10 +2049,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>27998</v>
@@ -2090,10 +2084,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>29721</v>
@@ -2125,10 +2119,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10">
         <v>27255</v>
@@ -2160,10 +2154,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>29721</v>
@@ -2195,10 +2189,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>30788</v>
@@ -2230,10 +2224,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>29721</v>
@@ -2265,10 +2259,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>27994</v>
@@ -2313,7 +2307,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2325,7 +2319,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2333,7 +2327,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -2348,24 +2342,24 @@
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>29241</v>
@@ -2397,10 +2391,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4">
         <v>26826</v>
@@ -2432,10 +2426,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>26826</v>
@@ -2467,10 +2461,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>29254</v>
@@ -2502,10 +2496,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>29254</v>
@@ -2537,10 +2531,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>30302</v>
@@ -2572,10 +2566,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>29216</v>
@@ -2607,10 +2601,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10">
         <v>26839</v>
@@ -2642,10 +2636,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>27553</v>
@@ -2677,10 +2671,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>27554</v>
@@ -2712,10 +2706,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13">
         <v>29254</v>
@@ -2747,10 +2741,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14">
         <v>29215</v>
@@ -2794,8 +2788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100436D0-0C8E-F840-A206-642D9CAB40B8}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2806,7 +2800,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2814,13 +2808,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
@@ -2829,24 +2823,24 @@
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>24757</v>
@@ -2878,10 +2872,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>26251</v>
@@ -2913,10 +2907,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>24110</v>
@@ -2948,10 +2942,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>26289</v>
@@ -2983,10 +2977,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>26289</v>
@@ -3018,10 +3012,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>24754</v>
@@ -3053,10 +3047,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>26289</v>
@@ -3088,10 +3082,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>27231</v>
@@ -3123,10 +3117,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>24098</v>
@@ -3158,10 +3152,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>24758</v>
@@ -3193,10 +3187,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>26275</v>
@@ -3228,10 +3222,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14">
         <v>24098</v>
@@ -3263,7 +3257,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3275,7 +3269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01401936-CB1F-E444-BF32-C06407CF4153}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K3:K14"/>
     </sheetView>
   </sheetViews>
@@ -3288,7 +3282,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -3296,7 +3290,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
@@ -3314,24 +3308,24 @@
         <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <v>29721</v>
@@ -3366,10 +3360,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4">
         <v>27255</v>
@@ -3404,10 +3398,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>29721</v>
@@ -3442,10 +3436,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>27997</v>
@@ -3480,10 +3474,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>27255</v>
@@ -3518,10 +3512,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>29682</v>
@@ -3556,10 +3550,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>30788</v>
@@ -3594,10 +3588,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>27998</v>
@@ -3632,10 +3626,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>27994</v>
@@ -3670,10 +3664,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>27268</v>
@@ -3708,10 +3702,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13">
         <v>29721</v>
@@ -3746,10 +3740,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>29708</v>
@@ -3787,7 +3781,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>